<commit_message>
remove some private information and added bayesian forecasting including the prophet algorithm
</commit_message>
<xml_diff>
--- a/github student information.xlsx
+++ b/github student information.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="123">
   <si>
     <t>Student Email</t>
   </si>
@@ -371,13 +371,22 @@
   </si>
   <si>
     <t>rmeehan03</t>
+  </si>
+  <si>
+    <t>etully02@qub.ac.uk</t>
+  </si>
+  <si>
+    <t>ellentully</t>
+  </si>
+  <si>
+    <t>Samitraj</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -428,7 +437,6 @@
       <color rgb="FF212121"/>
       <name val="-apple-system"/>
     </font>
-    <font/>
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -489,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -526,10 +534,7 @@
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -1338,7 +1343,7 @@
       <c r="A41" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="5" t="s">
         <v>73</v>
       </c>
       <c r="C41" s="4"/>
@@ -1425,7 +1430,7 @@
       <c r="A47" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="12" t="s">
         <v>84</v>
       </c>
       <c r="C47" s="4"/>
@@ -1440,7 +1445,7 @@
       <c r="A48" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="B48" s="5" t="s">
         <v>86</v>
       </c>
       <c r="C48" s="4"/>
@@ -1638,7 +1643,7 @@
       <c r="A62" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="13" t="s">
         <v>110</v>
       </c>
       <c r="C62" s="4"/>
@@ -1720,6 +1725,22 @@
       </c>
       <c r="B68" s="5" t="s">
         <v>119</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>